<commit_message>
11/17 updates for data sheet
</commit_message>
<xml_diff>
--- a/data/negative_cleanup.xlsx
+++ b/data/negative_cleanup.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rsong_admin\Box Sync\classes\cs273\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\cs273\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,21 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="281">
   <si>
     <t>nitromethane</t>
   </si>
   <si>
     <t>nitric acid</t>
-  </si>
-  <si>
-    <t>Product</t>
-  </si>
-  <si>
-    <t>Reactant</t>
-  </si>
-  <si>
-    <t>Sentences</t>
   </si>
   <si>
     <t>cyclohexanone oxime is an organic compound containing the functional group oxime.</t>
@@ -1211,10 +1202,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W67"/>
+  <dimension ref="A1:W66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,24 +1216,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1253,7 +1244,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1294,18 +1285,18 @@
         <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
@@ -1327,9 +1318,12 @@
         <v>26</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
         <v>27</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1338,12 +1332,9 @@
         <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1357,122 +1348,125 @@
       <c r="C12" t="s">
         <v>34</v>
       </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
         <v>39</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" t="s">
         <v>44</v>
       </c>
-      <c r="C15" t="s">
-        <v>42</v>
+      <c r="D15" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
         <v>50</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>51</v>
-      </c>
-      <c r="D17" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="C18" t="s">
         <v>53</v>
       </c>
-      <c r="D18" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" t="s">
         <v>58</v>
       </c>
-      <c r="C19" t="s">
-        <v>56</v>
+      <c r="D19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>60</v>
+      <c r="A20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="C20" t="s">
         <v>61</v>
       </c>
-      <c r="D20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="D21" t="s">
         <v>66</v>
-      </c>
-      <c r="C21" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1480,35 +1474,32 @@
         <v>67</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" t="s">
         <v>70</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" t="s">
         <v>75</v>
-      </c>
-      <c r="C24" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1527,84 +1518,84 @@
         <v>79</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" t="s">
         <v>80</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>81</v>
+      </c>
+      <c r="E26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" t="s">
+        <v>83</v>
+      </c>
+      <c r="G26" t="s">
+        <v>84</v>
+      </c>
+      <c r="H26" t="s">
+        <v>85</v>
+      </c>
+      <c r="I26" t="s">
+        <v>86</v>
+      </c>
+      <c r="J26" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>75</v>
+        <v>16</v>
       </c>
       <c r="C27" t="s">
-        <v>83</v>
-      </c>
-      <c r="D27" t="s">
-        <v>84</v>
-      </c>
-      <c r="E27" t="s">
-        <v>85</v>
-      </c>
-      <c r="F27" t="s">
-        <v>86</v>
-      </c>
-      <c r="G27" t="s">
-        <v>87</v>
-      </c>
-      <c r="H27" t="s">
-        <v>88</v>
-      </c>
-      <c r="I27" t="s">
         <v>89</v>
-      </c>
-      <c r="J27" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>92</v>
+      </c>
+      <c r="E28" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>19</v>
+        <v>95</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C29" t="s">
         <v>94</v>
       </c>
       <c r="D29" t="s">
-        <v>95</v>
-      </c>
-      <c r="E29" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" t="s">
         <v>98</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C30" t="s">
-        <v>97</v>
-      </c>
-      <c r="D30" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1617,70 +1608,73 @@
       <c r="C31" t="s">
         <v>101</v>
       </c>
+      <c r="D31" t="s">
+        <v>104</v>
+      </c>
+      <c r="E31" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" t="s">
+        <v>106</v>
+      </c>
+      <c r="G31" t="s">
+        <v>107</v>
+      </c>
+      <c r="I31" t="s">
+        <v>108</v>
+      </c>
+      <c r="J31" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
-      </c>
-      <c r="D32" t="s">
-        <v>107</v>
-      </c>
-      <c r="E32" t="s">
-        <v>108</v>
-      </c>
-      <c r="F32" t="s">
-        <v>109</v>
-      </c>
-      <c r="G32" t="s">
         <v>110</v>
-      </c>
-      <c r="I32" t="s">
-        <v>111</v>
-      </c>
-      <c r="J32" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" t="s">
         <v>115</v>
       </c>
-      <c r="C33" t="s">
-        <v>113</v>
+      <c r="E33" t="s">
+        <v>116</v>
+      </c>
+      <c r="F33" t="s">
+        <v>117</v>
+      </c>
+      <c r="G33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H33" t="s">
+        <v>119</v>
+      </c>
+      <c r="I33" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>117</v>
+        <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>118</v>
-      </c>
-      <c r="E34" t="s">
-        <v>119</v>
-      </c>
-      <c r="F34" t="s">
-        <v>120</v>
-      </c>
-      <c r="G34" t="s">
-        <v>121</v>
-      </c>
-      <c r="H34" t="s">
         <v>122</v>
       </c>
-      <c r="I34" t="s">
+      <c r="D34" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1689,7 +1683,7 @@
         <v>124</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>15</v>
+        <v>114</v>
       </c>
       <c r="C35" t="s">
         <v>125</v>
@@ -1697,24 +1691,21 @@
       <c r="D35" t="s">
         <v>126</v>
       </c>
+      <c r="E35" t="s">
+        <v>127</v>
+      </c>
+      <c r="F35" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="C36" t="s">
-        <v>128</v>
-      </c>
-      <c r="D36" t="s">
-        <v>129</v>
-      </c>
-      <c r="E36" t="s">
-        <v>130</v>
-      </c>
-      <c r="F36" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1728,21 +1719,21 @@
       <c r="C37" t="s">
         <v>134</v>
       </c>
+      <c r="D37" t="s">
+        <v>135</v>
+      </c>
+      <c r="E37" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C38" t="s">
-        <v>137</v>
-      </c>
-      <c r="D38" t="s">
-        <v>138</v>
-      </c>
-      <c r="E38" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1756,30 +1747,30 @@
       <c r="C39" t="s">
         <v>142</v>
       </c>
+      <c r="D39" t="s">
+        <v>143</v>
+      </c>
+      <c r="E39" t="s">
+        <v>144</v>
+      </c>
+      <c r="F39" t="s">
+        <v>145</v>
+      </c>
+      <c r="G39" t="s">
+        <v>146</v>
+      </c>
+      <c r="H39" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C40" t="s">
-        <v>145</v>
-      </c>
-      <c r="D40" t="s">
-        <v>146</v>
-      </c>
-      <c r="E40" t="s">
-        <v>147</v>
-      </c>
-      <c r="F40" t="s">
-        <v>148</v>
-      </c>
-      <c r="G40" t="s">
-        <v>149</v>
-      </c>
-      <c r="H40" t="s">
         <v>150</v>
       </c>
     </row>
@@ -1804,164 +1795,164 @@
       <c r="C42" t="s">
         <v>156</v>
       </c>
+      <c r="D42" t="s">
+        <v>157</v>
+      </c>
+      <c r="E42" t="s">
+        <v>158</v>
+      </c>
+      <c r="F42" t="s">
+        <v>159</v>
+      </c>
+      <c r="G42" t="s">
+        <v>160</v>
+      </c>
+      <c r="H42" t="s">
+        <v>161</v>
+      </c>
+      <c r="I42" t="s">
+        <v>162</v>
+      </c>
+      <c r="J42" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>158</v>
+        <v>57</v>
       </c>
       <c r="C43" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="D43" t="s">
-        <v>160</v>
-      </c>
-      <c r="E43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F43" t="s">
-        <v>162</v>
-      </c>
-      <c r="G43" t="s">
-        <v>163</v>
-      </c>
-      <c r="H43" t="s">
-        <v>164</v>
-      </c>
-      <c r="I43" t="s">
-        <v>165</v>
-      </c>
-      <c r="J43" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C44" t="s">
         <v>168</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C44" t="s">
-        <v>167</v>
       </c>
       <c r="D44" t="s">
         <v>169</v>
       </c>
+      <c r="E44" t="s">
+        <v>170</v>
+      </c>
+      <c r="F44" t="s">
+        <v>171</v>
+      </c>
+      <c r="G44" t="s">
+        <v>172</v>
+      </c>
+      <c r="H44" t="s">
+        <v>173</v>
+      </c>
+      <c r="I44" t="s">
+        <v>174</v>
+      </c>
+      <c r="J44" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>117</v>
+        <v>177</v>
       </c>
       <c r="C45" t="s">
-        <v>171</v>
-      </c>
-      <c r="D45" t="s">
-        <v>172</v>
-      </c>
-      <c r="E45" t="s">
-        <v>173</v>
-      </c>
-      <c r="F45" t="s">
-        <v>174</v>
-      </c>
-      <c r="G45" t="s">
-        <v>175</v>
-      </c>
-      <c r="H45" t="s">
-        <v>176</v>
-      </c>
-      <c r="I45" t="s">
-        <v>177</v>
-      </c>
-      <c r="J45" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" t="s">
         <v>179</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="D46" t="s">
         <v>180</v>
       </c>
-      <c r="C46" t="s">
+      <c r="E46" t="s">
         <v>181</v>
+      </c>
+      <c r="F46" t="s">
+        <v>182</v>
+      </c>
+      <c r="G46" t="s">
+        <v>183</v>
+      </c>
+      <c r="H46" t="s">
+        <v>184</v>
+      </c>
+      <c r="I46" t="s">
+        <v>185</v>
+      </c>
+      <c r="J46" t="s">
+        <v>186</v>
+      </c>
+      <c r="K46" t="s">
+        <v>187</v>
+      </c>
+      <c r="L46" t="s">
+        <v>188</v>
+      </c>
+      <c r="M46" t="s">
+        <v>189</v>
+      </c>
+      <c r="N46" t="s">
+        <v>190</v>
+      </c>
+      <c r="O46" t="s">
+        <v>191</v>
+      </c>
+      <c r="P46" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>193</v>
+      </c>
+      <c r="R46" t="s">
+        <v>194</v>
+      </c>
+      <c r="S46" t="s">
+        <v>195</v>
+      </c>
+      <c r="T46" t="s">
+        <v>196</v>
+      </c>
+      <c r="U46" t="s">
+        <v>197</v>
+      </c>
+      <c r="V46" t="s">
+        <v>198</v>
+      </c>
+      <c r="W46" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>60</v>
+        <v>200</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>15</v>
+        <v>201</v>
       </c>
       <c r="C47" t="s">
-        <v>182</v>
-      </c>
-      <c r="D47" t="s">
-        <v>183</v>
-      </c>
-      <c r="E47" t="s">
-        <v>184</v>
-      </c>
-      <c r="F47" t="s">
-        <v>185</v>
-      </c>
-      <c r="G47" t="s">
-        <v>186</v>
-      </c>
-      <c r="H47" t="s">
-        <v>187</v>
-      </c>
-      <c r="I47" t="s">
-        <v>188</v>
-      </c>
-      <c r="J47" t="s">
-        <v>189</v>
-      </c>
-      <c r="K47" t="s">
-        <v>190</v>
-      </c>
-      <c r="L47" t="s">
-        <v>191</v>
-      </c>
-      <c r="M47" t="s">
-        <v>192</v>
-      </c>
-      <c r="N47" t="s">
-        <v>193</v>
-      </c>
-      <c r="O47" t="s">
-        <v>194</v>
-      </c>
-      <c r="P47" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>196</v>
-      </c>
-      <c r="R47" t="s">
-        <v>197</v>
-      </c>
-      <c r="S47" t="s">
-        <v>198</v>
-      </c>
-      <c r="T47" t="s">
-        <v>199</v>
-      </c>
-      <c r="U47" t="s">
-        <v>200</v>
-      </c>
-      <c r="V47" t="s">
-        <v>201</v>
-      </c>
-      <c r="W47" t="s">
         <v>202</v>
       </c>
     </row>
@@ -1981,18 +1972,18 @@
         <v>206</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C49" t="s">
         <v>207</v>
       </c>
-      <c r="C49" t="s">
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="B50" t="s">
         <v>209</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="C50" t="s">
         <v>210</v>
@@ -2003,9 +1994,12 @@
         <v>211</v>
       </c>
       <c r="B51" t="s">
+        <v>102</v>
+      </c>
+      <c r="C51" t="s">
         <v>212</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>213</v>
       </c>
     </row>
@@ -2014,7 +2008,7 @@
         <v>214</v>
       </c>
       <c r="B52" t="s">
-        <v>105</v>
+        <v>57</v>
       </c>
       <c r="C52" t="s">
         <v>215</v>
@@ -2022,137 +2016,134 @@
       <c r="D52" t="s">
         <v>216</v>
       </c>
+      <c r="E52" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B53" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="C53" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D53" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E53" t="s">
-        <v>220</v>
+        <v>221</v>
+      </c>
+      <c r="F53" t="s">
+        <v>222</v>
+      </c>
+      <c r="G53" t="s">
+        <v>223</v>
+      </c>
+      <c r="H53" t="s">
+        <v>224</v>
+      </c>
+      <c r="I53" t="s">
+        <v>225</v>
+      </c>
+      <c r="J53" t="s">
+        <v>226</v>
+      </c>
+      <c r="K53" t="s">
+        <v>227</v>
+      </c>
+      <c r="L53" t="s">
+        <v>228</v>
+      </c>
+      <c r="M53" t="s">
+        <v>229</v>
+      </c>
+      <c r="N53" t="s">
+        <v>230</v>
+      </c>
+      <c r="O53" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="B54" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="C54" t="s">
-        <v>222</v>
-      </c>
-      <c r="D54" t="s">
-        <v>223</v>
-      </c>
-      <c r="E54" t="s">
-        <v>224</v>
-      </c>
-      <c r="F54" t="s">
-        <v>225</v>
-      </c>
-      <c r="G54" t="s">
-        <v>226</v>
-      </c>
-      <c r="H54" t="s">
-        <v>227</v>
-      </c>
-      <c r="I54" t="s">
-        <v>228</v>
-      </c>
-      <c r="J54" t="s">
-        <v>229</v>
-      </c>
-      <c r="K54" t="s">
-        <v>230</v>
-      </c>
-      <c r="L54" t="s">
-        <v>231</v>
-      </c>
-      <c r="M54" t="s">
         <v>232</v>
-      </c>
-      <c r="N54" t="s">
-        <v>233</v>
-      </c>
-      <c r="O54" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>235</v>
+      </c>
+      <c r="B55" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" t="s">
+        <v>234</v>
+      </c>
+      <c r="D55" t="s">
         <v>236</v>
       </c>
-      <c r="B55" t="s">
-        <v>58</v>
-      </c>
-      <c r="C55" t="s">
-        <v>235</v>
+      <c r="E55" t="s">
+        <v>237</v>
+      </c>
+      <c r="F55" t="s">
+        <v>238</v>
+      </c>
+      <c r="G55" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B56" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="C56" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D56" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="E56" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="F56" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="G56" t="s">
-        <v>242</v>
+        <v>245</v>
+      </c>
+      <c r="H56" t="s">
+        <v>246</v>
+      </c>
+      <c r="I56" t="s">
+        <v>247</v>
+      </c>
+      <c r="J56" t="s">
+        <v>248</v>
+      </c>
+      <c r="K56" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="B57" t="s">
-        <v>44</v>
+        <v>251</v>
       </c>
       <c r="C57" t="s">
-        <v>243</v>
-      </c>
-      <c r="D57" t="s">
-        <v>245</v>
-      </c>
-      <c r="E57" t="s">
-        <v>246</v>
-      </c>
-      <c r="F57" t="s">
-        <v>247</v>
-      </c>
-      <c r="G57" t="s">
-        <v>248</v>
-      </c>
-      <c r="H57" t="s">
-        <v>249</v>
-      </c>
-      <c r="I57" t="s">
-        <v>250</v>
-      </c>
-      <c r="J57" t="s">
-        <v>251</v>
-      </c>
-      <c r="K57" t="s">
         <v>252</v>
       </c>
     </row>
@@ -2161,18 +2152,18 @@
         <v>253</v>
       </c>
       <c r="B58" t="s">
+        <v>74</v>
+      </c>
+      <c r="C58" t="s">
         <v>254</v>
-      </c>
-      <c r="C58" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>255</v>
+      </c>
+      <c r="B59" t="s">
         <v>256</v>
-      </c>
-      <c r="B59" t="s">
-        <v>77</v>
       </c>
       <c r="C59" t="s">
         <v>257</v>
@@ -2180,13 +2171,13 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>259</v>
+      </c>
+      <c r="B60" t="s">
+        <v>260</v>
+      </c>
+      <c r="C60" t="s">
         <v>258</v>
-      </c>
-      <c r="B60" t="s">
-        <v>259</v>
-      </c>
-      <c r="C60" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
@@ -2221,33 +2212,36 @@
       <c r="C63" t="s">
         <v>267</v>
       </c>
+      <c r="D63" t="s">
+        <v>270</v>
+      </c>
+      <c r="E63" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>271</v>
+        <v>209</v>
       </c>
       <c r="B64" t="s">
+        <v>273</v>
+      </c>
+      <c r="C64" t="s">
         <v>272</v>
-      </c>
-      <c r="C64" t="s">
-        <v>270</v>
-      </c>
-      <c r="D64" t="s">
-        <v>273</v>
-      </c>
-      <c r="E64" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>212</v>
+        <v>275</v>
       </c>
       <c r="B65" t="s">
+        <v>155</v>
+      </c>
+      <c r="C65" t="s">
+        <v>274</v>
+      </c>
+      <c r="D65" t="s">
         <v>276</v>
-      </c>
-      <c r="C65" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2255,27 +2249,13 @@
         <v>278</v>
       </c>
       <c r="B66" t="s">
-        <v>158</v>
+        <v>279</v>
       </c>
       <c r="C66" t="s">
         <v>277</v>
       </c>
       <c r="D66" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>281</v>
-      </c>
-      <c r="B67" t="s">
-        <v>282</v>
-      </c>
-      <c r="C67" t="s">
         <v>280</v>
-      </c>
-      <c r="D67" t="s">
-        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>